<commit_message>
Add Sheet2Searcher utility and enhance By_Stage and PreProcessingPipeLine for improved data handling
</commit_message>
<xml_diff>
--- a/data/magdi reports.xlsx
+++ b/data/magdi reports.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29406"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1dc152c07513850c/Documents/GitHub/DataAnalyzer/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Excel Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{DE48D640-3B32-4E96-A8FC-C031BF16E8F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD2BB6A1-F648-4EA3-9D93-158D578B7169}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{DE48D640-3B32-4E96-A8FC-C031BF16E8F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD667EC9-24CE-45EC-AA73-568AB8634B4E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="599" firstSheet="1" activeTab="2" xr2:uid="{D0D76AE6-8D3C-4E35-ACCF-21D60420B679}"/>
   </bookViews>
@@ -17,11 +17,22 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -201,7 +212,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -502,10 +513,6 @@
 </inkml:ink>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4F4A3DED-29E2-4B29-9D9C-910E4B547F98}" name="Table1" displayName="Table1" ref="A1:O88" totalsRowShown="0">
   <autoFilter ref="A1:O88" xr:uid="{4F4A3DED-29E2-4B29-9D9C-910E4B547F98}"/>
@@ -569,8 +576,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A9F390E0-1750-489C-8911-003E3D324F7B}" name="Meeting_Table" displayName="Meeting_Table" ref="A1:B4" totalsRowShown="0">
-  <autoFilter ref="A1:B4" xr:uid="{A9F390E0-1750-489C-8911-003E3D324F7B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A9F390E0-1750-489C-8911-003E3D324F7B}" name="Meeting_Table" displayName="Meeting_Table" ref="A1:B2" totalsRowShown="0">
+  <autoFilter ref="A1:B2" xr:uid="{A9F390E0-1750-489C-8911-003E3D324F7B}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{0FB68F39-2F12-428E-9822-778005116B34}" name="Company Name"/>
     <tableColumn id="2" xr3:uid="{B7628F6C-9988-4BFE-957C-8B3F841E2B09}" name="Meeting Date"/>
@@ -580,8 +587,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{40104921-C41E-428D-BDE7-743972A8F27B}" name="Calls_Table" displayName="Calls_Table" ref="G1:H4" totalsRowShown="0">
-  <autoFilter ref="G1:H4" xr:uid="{40104921-C41E-428D-BDE7-743972A8F27B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{40104921-C41E-428D-BDE7-743972A8F27B}" name="Calls_Table" displayName="Calls_Table" ref="G1:H2" totalsRowShown="0">
+  <autoFilter ref="G1:H2" xr:uid="{40104921-C41E-428D-BDE7-743972A8F27B}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{B63E79F1-8B43-452F-B306-3D08DB1AE2F9}" name="Number of Calles"/>
     <tableColumn id="2" xr3:uid="{F542CCFF-F4BE-42C2-B3D5-BE891327A23D}" name="Calls Date"/>
@@ -591,9 +598,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -631,7 +638,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -737,7 +744,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -879,7 +886,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -893,24 +900,24 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="3" width="20.88671875" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" customWidth="1"/>
-    <col min="5" max="5" width="37.44140625" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" customWidth="1"/>
-    <col min="8" max="8" width="24.33203125" customWidth="1"/>
-    <col min="9" max="9" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.109375" customWidth="1"/>
-    <col min="11" max="11" width="17.5546875" customWidth="1"/>
-    <col min="12" max="12" width="17.88671875" customWidth="1"/>
-    <col min="13" max="13" width="16.6640625" customWidth="1"/>
-    <col min="14" max="14" width="18.44140625" customWidth="1"/>
-    <col min="15" max="15" width="16.6640625" customWidth="1"/>
+    <col min="1" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="5" max="5" width="37.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="8" max="8" width="24.28515625" customWidth="1"/>
+    <col min="9" max="9" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" customWidth="1"/>
+    <col min="12" max="12" width="17.85546875" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" customWidth="1"/>
+    <col min="14" max="14" width="18.42578125" customWidth="1"/>
+    <col min="15" max="15" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -957,7 +964,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15">
       <c r="A2">
         <v>10001</v>
       </c>
@@ -992,28 +999,28 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
     <col min="1" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="31.6640625" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" customWidth="1"/>
     <col min="4" max="9" width="21" customWidth="1"/>
-    <col min="10" max="10" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="21" customWidth="1"/>
-    <col min="14" max="16" width="21.109375" customWidth="1"/>
-    <col min="17" max="17" width="20.5546875" customWidth="1"/>
-    <col min="18" max="18" width="21.33203125" customWidth="1"/>
+    <col min="14" max="16" width="21.140625" customWidth="1"/>
+    <col min="17" max="17" width="20.5703125" customWidth="1"/>
+    <col min="18" max="18" width="21.28515625" customWidth="1"/>
     <col min="19" max="19" width="22" customWidth="1"/>
-    <col min="20" max="20" width="16.109375" customWidth="1"/>
-    <col min="21" max="21" width="16.88671875" customWidth="1"/>
-    <col min="22" max="22" width="17.6640625" customWidth="1"/>
-    <col min="23" max="23" width="14.44140625" customWidth="1"/>
-    <col min="24" max="24" width="14.6640625" customWidth="1"/>
-    <col min="25" max="25" width="22.6640625" customWidth="1"/>
-    <col min="26" max="26" width="23.33203125" customWidth="1"/>
-    <col min="27" max="27" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.140625" customWidth="1"/>
+    <col min="21" max="21" width="16.85546875" customWidth="1"/>
+    <col min="22" max="22" width="17.7109375" customWidth="1"/>
+    <col min="23" max="23" width="14.42578125" customWidth="1"/>
+    <col min="24" max="24" width="14.7109375" customWidth="1"/>
+    <col min="25" max="25" width="22.7109375" customWidth="1"/>
+    <col min="26" max="26" width="23.28515625" customWidth="1"/>
+    <col min="27" max="27" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1096,7 +1103,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" ht="15.6" customHeight="1">
       <c r="A2">
         <v>10001</v>
       </c>
@@ -1156,7 +1163,7 @@
       <c r="AA2" s="3"/>
       <c r="AB2" s="1"/>
     </row>
-    <row r="3" spans="1:28" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" ht="16.899999999999999" customHeight="1">
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
@@ -1169,49 +1176,49 @@
       <c r="AA3" s="3"/>
       <c r="AB3" s="1"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28">
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
       <c r="Z5" s="3"/>
       <c r="AA5" s="3"/>
       <c r="AB5" s="1"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28">
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
       <c r="Z6" s="3"/>
       <c r="AA6" s="3"/>
       <c r="AB6" s="1"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28">
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
       <c r="Z7" s="3"/>
       <c r="AA7" s="3"/>
       <c r="AB7" s="1"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28">
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
       <c r="Z8" s="3"/>
       <c r="AA8" s="3"/>
       <c r="AB8" s="1"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28">
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
       <c r="Z9" s="3"/>
       <c r="AA9" s="3"/>
       <c r="AB9" s="1"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28">
       <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
       <c r="Z10" s="3"/>
       <c r="AA10" s="3"/>
       <c r="AB10" s="1"/>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:1">
       <c r="A89" t="s">
         <v>51</v>
       </c>
@@ -1240,21 +1247,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3A4C288-A87C-49B3-B1E5-1AA21A4B10B3}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="A3:H4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -1268,7 +1275,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1281,14 +1288,6 @@
       <c r="H2" s="5">
         <v>45945</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="5"/>
-      <c r="H3" s="5"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="5"/>
-      <c r="H4" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>